<commit_message>
datos de openacc en el excel
</commit_message>
<xml_diff>
--- a/CHALLENGE/scalability-results.xlsx
+++ b/CHALLENGE/scalability-results.xlsx
@@ -252,7 +252,7 @@
   <dimension ref="A1:G27"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="145" zoomScaleNormal="145" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E27" activeCellId="0" sqref="E27"/>
+      <selection pane="topLeft" activeCell="G28" activeCellId="0" sqref="G28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -509,6 +509,12 @@
       </c>
       <c r="E27" s="0" t="n">
         <v>618.34</v>
+      </c>
+      <c r="F27" s="0" t="n">
+        <v>972.2</v>
+      </c>
+      <c r="G27" s="0" t="n">
+        <v>1735.14</v>
       </c>
     </row>
   </sheetData>

</xml_diff>